<commit_message>
Checking in all newly added tests and modified files.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/CheckRNAiTabInGF.xlsx
+++ b/src/main/resources/testdata/CheckRNAiTabInGF.xlsx
@@ -117,7 +117,7 @@
     <t>selenium_assession</t>
   </si>
   <si>
-    <t>1 caagtgccac tggctactag tgcaagtatg gctcgggtct ctgccaatgc agttgcactt
+    <t xml:space="preserve">1 caagtgccac tggctactag tgcaagtatg gctcgggtct ctgccaatgc agttgcactt
        61 gttgcactcg tctccgttct tctcacgtat ggctgctgcg cccagtcgcc gctcaactac
       121 accggctcct tggccaaatc ctccaaggct agctggtcat ggctccctgc caaggccaca
       181 tggtacggcg cgcctaccgg cgccggtccc gatgacaacg gtggtgcttg cggctacaag
@@ -132,7 +132,7 @@
       721 aggcgccggc tgcagggccc cttctctctc cgcatccgca gcgaatccgg caagacgctg
       781 gtggccaaac aagtcatccc ggccaactgg aggcccgaca cgaactaccg ttccaacgtc
       841 cagttccgtt gattgctccg agcttccgat cgatcgacga agacgttgat taattcgg
-amakpgqndk lrhagiidiq  fqrvpcnhpg lnvnfqverg 181 snpnylavlv efanregtvv qmdlmesrng rptgywtamr hswgaiwrmd srrrlqgpfs 241 lrirsesgkt lvakqvipan wrpdtnyrsn vqfr</t>
+</t>
   </si>
 </sst>
 </file>
@@ -476,18 +476,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="28.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="255.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>